<commit_message>
updates to excel file for sql planning. added more details for table outline
</commit_message>
<xml_diff>
--- a/SQL_DB_Planning/RecipEasy Relational Database Tables.xlsx
+++ b/SQL_DB_Planning/RecipEasy Relational Database Tables.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b75816bd0ef4506b/Documents/School Notes/CU Boulder-CompSci Notes/2024 Spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elainefrench/Documents/3308/3308_Team3_Project/SQL_DB_Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="189" documentId="8_{3BB74AF3-AEAF-43A3-8AB1-88E5CF7B5B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BCBD802-1E98-484A-8E6F-3E1E72D26299}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7699838-16C1-4942-99EE-9A76D9BCF06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4D5B498A-86E9-4F80-B29B-28BFEB12C9C0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{4D5B498A-86E9-4F80-B29B-28BFEB12C9C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table Descriptions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="71">
   <si>
     <t>Recipies</t>
   </si>
@@ -156,13 +156,106 @@
   </si>
   <si>
     <t>Am I missing anything???</t>
+  </si>
+  <si>
+    <t>Recipe_Table</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Field name</t>
+  </si>
+  <si>
+    <t>Recipe_ID</t>
+  </si>
+  <si>
+    <t>Recipe Name</t>
+  </si>
+  <si>
+    <t>Serving Size</t>
+  </si>
+  <si>
+    <t>Cook Time</t>
+  </si>
+  <si>
+    <t>Cooking Instructions</t>
+  </si>
+  <si>
+    <t>Average User Rating</t>
+  </si>
+  <si>
+    <t>User_Table</t>
+  </si>
+  <si>
+    <t>User_ID</t>
+  </si>
+  <si>
+    <t>Community_Table</t>
+  </si>
+  <si>
+    <t>User name</t>
+  </si>
+  <si>
+    <t>Post_ID</t>
+  </si>
+  <si>
+    <t>Post Title</t>
+  </si>
+  <si>
+    <t>User Rating</t>
+  </si>
+  <si>
+    <t>Post Date</t>
+  </si>
+  <si>
+    <t>UTC</t>
+  </si>
+  <si>
+    <t>User Comments</t>
+  </si>
+  <si>
+    <t>User comments on the recipe; post content</t>
+  </si>
+  <si>
+    <t>short text</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>INT (len=1)</t>
+  </si>
+  <si>
+    <t>Float (len=2)</t>
+  </si>
+  <si>
+    <t>list of strings</t>
+  </si>
+  <si>
+    <t>INT (max len=3)</t>
+  </si>
+  <si>
+    <t>cookiing time in minutes (integers only)</t>
+  </si>
+  <si>
+    <t>long text</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>what about a route that is( '/recipe/&lt;recipe_name&gt;') -- and then the recipe_name variable is replace with the recipe name field from the recipes table</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,8 +295,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +331,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,23 +380,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,59 +744,59 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="121.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="119.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="121.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="119.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="91" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" ht="27" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -679,92 +813,88 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="F11" s="5" t="s">
+    <row r="11" spans="1:15" ht="18" x14ac:dyDescent="0.25">
+      <c r="F11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="F12" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="6" t="s">
         <v>22</v>
       </c>
       <c r="H12" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H13" t="s">
         <v>19</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" t="s">
         <v>33</v>
       </c>
-      <c r="J13" s="9"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F14" s="9" t="s">
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" t="s">
         <v>34</v>
       </c>
-      <c r="J14" s="9"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F15" s="9" t="s">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="9" t="s">
+      <c r="H15" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F16" s="9" t="s">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="9" t="s">
+      <c r="H16" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="9" t="s">
+      <c r="I16" t="s">
         <v>34</v>
       </c>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F17" t="s">
         <v>25</v>
       </c>
@@ -775,7 +905,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F18" t="s">
         <v>26</v>
       </c>
@@ -786,11 +916,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="8"/>
       <c r="F19" t="s">
         <v>27</v>
       </c>
@@ -801,7 +931,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -818,7 +948,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F21" t="s">
         <v>29</v>
       </c>
@@ -829,7 +959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F22" t="s">
         <v>37</v>
       </c>
@@ -840,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F23" t="s">
         <v>38</v>
       </c>
@@ -851,30 +981,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="F24" s="11" t="s">
+    <row r="24" spans="1:8" ht="20" x14ac:dyDescent="0.25">
+      <c r="F24" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="F28" s="6" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F25" s="15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F28" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="F29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>10</v>
       </c>
@@ -898,4 +1033,191 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD511AA3-F360-DC4B-8FBC-D6B9A75534EC}">
+  <dimension ref="A1:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="10" customWidth="1"/>
+    <col min="3" max="3" width="38" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="10"/>
+    <col min="5" max="5" width="11.83203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="10"/>
+    <col min="7" max="7" width="12.33203125" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="18.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="E1" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="I1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="I1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>